<commit_message>
improve report loa/str : FRO comments
</commit_message>
<xml_diff>
--- a/templates/Report Loa.xlsx
+++ b/templates/Report Loa.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F43FE38-6109-45B2-88BD-B91E29CCC9E2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55E80FD-E7EF-4458-9E0E-52E0CB450FA8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,9 +67,9 @@
     <definedName name="PV_Réf_éprouvette">#REF!</definedName>
     <definedName name="PV_Température">#REF!</definedName>
     <definedName name="PV_εmax_imposée">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Courbes!$A$1:$H$43</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'En-tête'!$A$1:$H$51</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">PV!$A$1:$D$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Courbes!$A$1:$H$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'En-tête'!$A$1:$H$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">PV!$A$1:$D$61</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>The results presented in this report relate only to the items tested</t>
-  </si>
-  <si>
-    <t>LOAD CONTROL</t>
   </si>
   <si>
     <t>Date</t>
@@ -420,39 +417,12 @@
     <t>Rev :</t>
   </si>
   <si>
-    <t xml:space="preserve">N° du Projet :  </t>
-  </si>
-  <si>
-    <t>Type d'Essai :</t>
-  </si>
-  <si>
-    <t>Référence Matière :</t>
-  </si>
-  <si>
-    <t>Nombre d'Eprouvette :</t>
-  </si>
-  <si>
-    <t>Nombre d'Essais :</t>
-  </si>
-  <si>
     <t xml:space="preserve">Origine : </t>
   </si>
   <si>
-    <t>Référence d'Usinage :</t>
-  </si>
-  <si>
-    <t>Specification d'Usinage ::</t>
-  </si>
-  <si>
-    <t>N° de Dessin :</t>
-  </si>
-  <si>
     <t>Contrôle Axial</t>
   </si>
   <si>
-    <t>Specification d'Essai :</t>
-  </si>
-  <si>
     <t>Signal :</t>
   </si>
   <si>
@@ -505,6 +475,36 @@
   </si>
   <si>
     <t>Cycle du dernier niveau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N° du projet :  </t>
+  </si>
+  <si>
+    <t>Type d'essai :</t>
+  </si>
+  <si>
+    <t>Référence matière :</t>
+  </si>
+  <si>
+    <t>Nombre d'essais :</t>
+  </si>
+  <si>
+    <t>Nombre d'eprouvette :</t>
+  </si>
+  <si>
+    <t>Référence d'usinage :</t>
+  </si>
+  <si>
+    <t>N° de dessin :</t>
+  </si>
+  <si>
+    <t>Specification d'essai :</t>
+  </si>
+  <si>
+    <t>Specification d'usinage :</t>
+  </si>
+  <si>
+    <t>CONTRÔLE EFFORT</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1130,7 @@
     <xf numFmtId="166" fontId="22" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1436,21 +1436,42 @@
     <xf numFmtId="49" fontId="4" fillId="6" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="5" borderId="23" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="5" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1472,20 +1493,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="5" borderId="23" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="24" fillId="5" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1494,7 +1503,17 @@
     <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1541,9 +1560,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>135321</xdr:rowOff>
+      <xdr:colOff>464306</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1574,7 +1593,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="742950" cy="744921"/>
+          <a:ext cx="911981" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1593,25 +1612,25 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>178575</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Image 4">
+        <xdr:cNvPr id="9" name="Image 11" descr="image001">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE378C59-7309-4BFB-800A-071B767C32E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3FBC55B-1BCA-4F17-B446-270035452779}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1620,7 +1639,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1634,13 +1653,16 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6067425" y="0"/>
-          <a:ext cx="371474" cy="1874025"/>
+          <a:off x="6181725" y="0"/>
+          <a:ext cx="409575" cy="2057400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
@@ -1648,6 +1670,16 @@
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -2057,13 +2089,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Feuil1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G11"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2075,39 +2107,39 @@
     <col min="5" max="5" width="11.140625" style="11" customWidth="1"/>
     <col min="6" max="6" width="17.140625" style="11" customWidth="1"/>
     <col min="7" max="7" width="4.5703125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" style="11" customWidth="1"/>
     <col min="9" max="10" width="10.7109375" style="11"/>
     <col min="11" max="13" width="10.7109375" style="11" hidden="1" customWidth="1"/>
     <col min="14" max="16384" width="10.7109375" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="133" t="s">
-        <v>125</v>
-      </c>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="130" t="s">
-        <v>33</v>
-      </c>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="137"/>
     </row>
     <row r="2" spans="1:8" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="130"/>
+      <c r="B2" s="135" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="137"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="133"/>
-      <c r="C3" s="133"/>
-      <c r="D3" s="133"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="133"/>
-      <c r="G3" s="130"/>
+      <c r="B3" s="136" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="136"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="137"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" s="17"/>
@@ -2115,42 +2147,42 @@
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
-      <c r="G4" s="130"/>
+      <c r="G4" s="137"/>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" s="19"/>
-      <c r="G5" s="130"/>
+      <c r="G5" s="137"/>
     </row>
     <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="18"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="G6" s="130"/>
+        <v>114</v>
+      </c>
+      <c r="G6" s="137"/>
     </row>
     <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="18"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
       <c r="E7" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" s="20"/>
-      <c r="G7" s="130"/>
+      <c r="G7" s="137"/>
     </row>
     <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="18"/>
@@ -2158,17 +2190,17 @@
       <c r="D8" s="17"/>
       <c r="E8" s="25"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="130"/>
+      <c r="G8" s="137"/>
     </row>
     <row r="9" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="18"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="25" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="F9" s="20"/>
-      <c r="G9" s="130"/>
+      <c r="G9" s="137"/>
     </row>
     <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="21"/>
@@ -2176,7 +2208,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="26"/>
       <c r="F10" s="22"/>
-      <c r="G10" s="130"/>
+      <c r="G10" s="137"/>
     </row>
     <row r="11" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="18"/>
@@ -2184,7 +2216,7 @@
       <c r="D11" s="17"/>
       <c r="E11" s="25"/>
       <c r="F11" s="23"/>
-      <c r="G11" s="130"/>
+      <c r="G11" s="137"/>
     </row>
     <row r="12" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="18"/>
@@ -2196,62 +2228,62 @@
     </row>
     <row r="13" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="141" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="134" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="135"/>
-      <c r="E13" s="135"/>
-      <c r="F13" s="135"/>
-      <c r="G13" s="135"/>
-      <c r="H13" s="136"/>
+      <c r="D13" s="142"/>
+      <c r="E13" s="142"/>
+      <c r="F13" s="142"/>
+      <c r="G13" s="142"/>
+      <c r="H13" s="143"/>
     </row>
     <row r="14" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="35"/>
       <c r="B14" s="36"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="137"/>
-      <c r="E14" s="137"/>
-      <c r="F14" s="137"/>
-      <c r="G14" s="137"/>
-      <c r="H14" s="137"/>
+      <c r="C14" s="144"/>
+      <c r="D14" s="144"/>
+      <c r="E14" s="144"/>
+      <c r="F14" s="144"/>
+      <c r="G14" s="144"/>
+      <c r="H14" s="144"/>
     </row>
     <row r="15" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="37"/>
       <c r="B15" s="38"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="138"/>
-      <c r="F15" s="138"/>
-      <c r="G15" s="138"/>
-      <c r="H15" s="138"/>
+      <c r="C15" s="145"/>
+      <c r="D15" s="145"/>
+      <c r="E15" s="145"/>
+      <c r="F15" s="145"/>
+      <c r="G15" s="145"/>
+      <c r="H15" s="145"/>
     </row>
     <row r="16" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="39"/>
       <c r="B16" s="38"/>
-      <c r="C16" s="139"/>
-      <c r="D16" s="139"/>
-      <c r="E16" s="139"/>
-      <c r="F16" s="139"/>
-      <c r="G16" s="139"/>
-      <c r="H16" s="139"/>
+      <c r="C16" s="146"/>
+      <c r="D16" s="146"/>
+      <c r="E16" s="146"/>
+      <c r="F16" s="146"/>
+      <c r="G16" s="146"/>
+      <c r="H16" s="146"/>
     </row>
     <row r="17" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="131" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="131"/>
-      <c r="C18" s="131"/>
-      <c r="D18" s="131"/>
-      <c r="E18" s="131"/>
-      <c r="F18" s="131"/>
-      <c r="G18" s="131"/>
-      <c r="H18" s="131"/>
+      <c r="A18" s="139" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="139"/>
+      <c r="C18" s="139"/>
+      <c r="D18" s="139"/>
+      <c r="E18" s="139"/>
+      <c r="F18" s="139"/>
+      <c r="G18" s="139"/>
+      <c r="H18" s="139"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
@@ -2262,38 +2294,38 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" s="140"/>
-      <c r="D20" s="140"/>
-      <c r="E20" s="140"/>
-      <c r="F20" s="140"/>
-      <c r="G20" s="140"/>
-      <c r="H20" s="140"/>
+        <v>92</v>
+      </c>
+      <c r="C20" s="147"/>
+      <c r="D20" s="147"/>
+      <c r="E20" s="147"/>
+      <c r="F20" s="147"/>
+      <c r="G20" s="147"/>
+      <c r="H20" s="147"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="C21" s="140"/>
-      <c r="D21" s="140"/>
-      <c r="E21" s="140"/>
-      <c r="F21" s="140"/>
-      <c r="G21" s="140"/>
-      <c r="H21" s="140"/>
+      <c r="C21" s="147"/>
+      <c r="D21" s="147"/>
+      <c r="E21" s="147"/>
+      <c r="F21" s="147"/>
+      <c r="G21" s="147"/>
+      <c r="H21" s="147"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="29" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="C22" s="14"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="29" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="16"/>
@@ -2303,7 +2335,7 @@
       <c r="A24" s="5"/>
       <c r="B24" s="30"/>
       <c r="C24" s="13" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="16"/>
@@ -2313,7 +2345,7 @@
       <c r="A25" s="5"/>
       <c r="B25" s="30"/>
       <c r="C25" s="13" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D25" s="13"/>
       <c r="E25" s="16"/>
@@ -2324,7 +2356,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="30"/>
       <c r="C26" s="13" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="16"/>
@@ -2343,7 +2375,7 @@
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="29" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="13"/>
@@ -2353,7 +2385,7 @@
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="31" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="13"/>
@@ -2363,7 +2395,7 @@
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="31" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="13"/>
@@ -2382,7 +2414,7 @@
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="30" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C32" s="13" t="str">
         <f>IF(K32=0,M32,L32)</f>
@@ -2393,17 +2425,17 @@
       <c r="F32" s="16"/>
       <c r="K32" s="91"/>
       <c r="L32" s="92" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="M32" s="93" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="N32" s="91"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
       <c r="B33" s="30" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -2413,7 +2445,7 @@
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="30" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -2423,7 +2455,7 @@
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="31" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="13"/>
@@ -2434,16 +2466,16 @@
       <c r="A36" s="5"/>
     </row>
     <row r="37" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="131" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="131"/>
-      <c r="C37" s="131"/>
-      <c r="D37" s="131"/>
-      <c r="E37" s="131"/>
-      <c r="F37" s="131"/>
-      <c r="G37" s="131"/>
-      <c r="H37" s="131"/>
+      <c r="A37" s="139" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="139"/>
+      <c r="C37" s="139"/>
+      <c r="D37" s="139"/>
+      <c r="E37" s="139"/>
+      <c r="F37" s="139"/>
+      <c r="G37" s="139"/>
+      <c r="H37" s="139"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
@@ -2451,13 +2483,13 @@
     <row r="39" spans="1:13" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
       <c r="B39" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="C39" s="132"/>
-      <c r="D39" s="132"/>
-      <c r="E39" s="132"/>
-      <c r="F39" s="132"/>
-      <c r="G39" s="132"/>
+        <v>127</v>
+      </c>
+      <c r="C39" s="140"/>
+      <c r="D39" s="140"/>
+      <c r="E39" s="140"/>
+      <c r="F39" s="140"/>
+      <c r="G39" s="140"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
@@ -2474,10 +2506,10 @@
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
       <c r="B41" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
@@ -2490,7 +2522,7 @@
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
       <c r="B42" s="31" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C42" s="13"/>
       <c r="D42" s="13" t="s">
@@ -2508,19 +2540,19 @@
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
       <c r="B43" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="129" t="str">
+        <v>103</v>
+      </c>
+      <c r="C43" s="138" t="str">
         <f>CONCATENATE("Système hydraulique de ",K43," kN avec servovalve contrôlé par une boucle d'asservissement.")</f>
         <v>Système hydraulique de xxx kN avec servovalve contrôlé par une boucle d'asservissement.</v>
       </c>
-      <c r="D43" s="129"/>
-      <c r="E43" s="129"/>
-      <c r="F43" s="129"/>
-      <c r="G43" s="129"/>
-      <c r="H43" s="129"/>
+      <c r="D43" s="138"/>
+      <c r="E43" s="138"/>
+      <c r="F43" s="138"/>
+      <c r="G43" s="138"/>
+      <c r="H43" s="138"/>
       <c r="K43" s="91" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L43" s="88"/>
       <c r="M43" s="88"/>
@@ -2528,7 +2560,7 @@
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
       <c r="B44" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C44" s="89"/>
       <c r="D44" s="13"/>
@@ -2542,10 +2574,10 @@
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
       <c r="B45" s="31" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C45" s="13" t="str">
-        <f>IF(AND(K45=0,L45=0),"NA",CONCATENATE(IF(K45&gt;0,"Furnace",""),IF(L45&gt;0,"Coil","")))</f>
+        <f>IF(AND(K45=0,L45=0),"NA",CONCATENATE(IF(K45&gt;0,"Four",""),IF(L45&gt;0,"Induction","")))</f>
         <v>NA</v>
       </c>
       <c r="D45" s="13"/>
@@ -2558,87 +2590,113 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="12"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="15"/>
       <c r="K46" s="88"/>
       <c r="L46" s="88"/>
       <c r="M46" s="88"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
-      <c r="B47" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="G47" s="5"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="15"/>
       <c r="K47" s="88"/>
       <c r="L47" s="88"/>
       <c r="M47" s="88"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="5"/>
-      <c r="B48" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G48" s="5"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="12"/>
+      <c r="K48" s="88"/>
+      <c r="L48" s="88"/>
+      <c r="M48" s="88"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
-      <c r="B49" s="8" t="s">
-        <v>115</v>
+      <c r="B49" s="28" t="s">
+        <v>37</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="8" t="s">
-        <v>116</v>
+      <c r="F49" s="28" t="s">
+        <v>37</v>
       </c>
       <c r="G49" s="5"/>
-    </row>
-    <row r="50" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
+      <c r="K49" s="88"/>
+      <c r="L49" s="88"/>
+      <c r="M49" s="88"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
+      <c r="B50" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" s="5"/>
+      <c r="B51" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="K50" s="6"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="148"/>
+      <c r="H52" s="148"/>
+      <c r="K52" s="6"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="148"/>
+      <c r="H53" s="148"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="9">
     <mergeCell ref="C43:H43"/>
-    <mergeCell ref="G1:G11"/>
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="A37:H37"/>
     <mergeCell ref="C39:G39"/>
-    <mergeCell ref="B1:F3"/>
     <mergeCell ref="C13:H13"/>
     <mergeCell ref="C14:H14"/>
     <mergeCell ref="C15:H15"/>
@@ -2646,23 +2704,31 @@
     <mergeCell ref="C20:H21"/>
   </mergeCells>
   <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$C$20=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$C$44=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$C$33=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$C$34=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="88" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;G</oddFooter>
   </headerFooter>
-  <colBreaks count="1" manualBreakCount="1">
-    <brk id="8" max="1048575" man="1"/>
-  </colBreaks>
   <drawing r:id="rId2"/>
   <legacyDrawingHF r:id="rId3"/>
 </worksheet>
@@ -2670,9 +2736,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Feuil2">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:CY76"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="D14" sqref="D14:D15"/>
       <selection pane="topRight" activeCell="D59" sqref="D59"/>
@@ -2688,7 +2757,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="94" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P1" s="95" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="41" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2696,7 +2765,7 @@
     </row>
     <row r="5" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="96" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="97"/>
       <c r="C5" s="98" t="s">
@@ -2706,7 +2775,7 @@
     </row>
     <row r="6" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="96" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="97"/>
       <c r="C6" s="98" t="s">
@@ -2716,7 +2785,7 @@
     </row>
     <row r="7" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="44"/>
       <c r="C7" s="46" t="s">
@@ -2726,7 +2795,7 @@
     </row>
     <row r="8" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="44"/>
       <c r="C8" s="48" t="s">
@@ -2736,7 +2805,7 @@
     </row>
     <row r="9" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="44"/>
       <c r="C9" s="48" t="s">
@@ -2754,38 +2823,38 @@
     </row>
     <row r="11" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="44"/>
       <c r="C11" s="51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="47"/>
     </row>
     <row r="12" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="44"/>
       <c r="C12" s="51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="47"/>
     </row>
     <row r="13" spans="1:16" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="44"/>
       <c r="C13" s="51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="47"/>
     </row>
     <row r="14" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="105"/>
       <c r="B14" s="106" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="107" t="s">
         <v>28</v>
@@ -2795,7 +2864,7 @@
     <row r="15" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="105"/>
       <c r="B15" s="106" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="107" t="s">
         <v>28</v>
@@ -2804,7 +2873,7 @@
     </row>
     <row r="16" spans="1:16" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="111" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B16" s="106"/>
       <c r="C16" s="107" t="s">
@@ -2814,7 +2883,7 @@
     </row>
     <row r="17" spans="1:4" ht="14.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="128" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B17" s="109"/>
       <c r="C17" s="127" t="str">
@@ -2825,7 +2894,7 @@
     </row>
     <row r="18" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="53"/>
       <c r="C18" s="54" t="s">
@@ -2835,41 +2904,41 @@
     </row>
     <row r="19" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="44"/>
       <c r="C19" s="51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" s="56"/>
     </row>
     <row r="20" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="44"/>
       <c r="C20" s="51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" s="56"/>
     </row>
     <row r="21" spans="1:4" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="58"/>
       <c r="C21" s="59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D21" s="60"/>
     </row>
     <row r="22" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="119" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="120"/>
       <c r="C22" s="121" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="122"/>
     </row>
@@ -2879,7 +2948,7 @@
       </c>
       <c r="B23" s="62"/>
       <c r="C23" s="51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="63"/>
     </row>
@@ -2897,99 +2966,99 @@
       </c>
       <c r="B25" s="64"/>
       <c r="C25" s="51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" s="63"/>
     </row>
     <row r="26" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="62"/>
       <c r="C26" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" s="65"/>
     </row>
     <row r="27" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="64"/>
       <c r="C27" s="51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" s="66"/>
     </row>
     <row r="28" spans="1:4" ht="14.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="68" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="58"/>
       <c r="C28" s="59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" s="123"/>
     </row>
     <row r="29" spans="1:4" ht="14.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="141" t="s">
-        <v>128</v>
-      </c>
-      <c r="B29" s="142"/>
-      <c r="C29" s="143"/>
-      <c r="D29" s="144"/>
+      <c r="A29" s="129" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="130"/>
+      <c r="C29" s="131"/>
+      <c r="D29" s="132"/>
     </row>
     <row r="30" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="124" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="125" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="125" t="s">
+      <c r="C30" s="54" t="s">
         <v>62</v>
-      </c>
-      <c r="C30" s="54" t="s">
-        <v>63</v>
       </c>
       <c r="D30" s="126"/>
     </row>
     <row r="31" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" s="67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D31" s="63"/>
     </row>
     <row r="32" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D32" s="63"/>
     </row>
     <row r="33" spans="1:4" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C33" s="59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D33" s="70"/>
     </row>
     <row r="34" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B34" s="53"/>
       <c r="C34" s="54"/>
@@ -2997,115 +3066,115 @@
     </row>
     <row r="35" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="62" t="s">
-        <v>69</v>
-      </c>
       <c r="C35" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D35" s="63"/>
     </row>
     <row r="36" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B36" s="64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D36" s="63"/>
     </row>
     <row r="37" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C37" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D37" s="63"/>
     </row>
     <row r="38" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38" s="62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C38" s="51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" s="65"/>
     </row>
     <row r="39" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="64" t="s">
+      <c r="C39" s="51" t="s">
         <v>74</v>
-      </c>
-      <c r="C39" s="51" t="s">
-        <v>75</v>
       </c>
       <c r="D39" s="66"/>
     </row>
     <row r="40" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B40" s="64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C40" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D40" s="71"/>
     </row>
     <row r="41" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B41" s="64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D41" s="71"/>
     </row>
     <row r="42" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B42" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C42" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D42" s="71"/>
     </row>
     <row r="43" spans="1:4" ht="14.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B43" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C43" s="59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D43" s="72"/>
     </row>
     <row r="44" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B44" s="53"/>
       <c r="C44" s="46"/>
@@ -3113,7 +3182,7 @@
     </row>
     <row r="45" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45" s="44"/>
       <c r="C45" s="48"/>
@@ -3121,7 +3190,7 @@
     </row>
     <row r="46" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B46" s="44"/>
       <c r="C46" s="48"/>
@@ -3129,7 +3198,7 @@
     </row>
     <row r="47" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="111" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B47" s="106"/>
       <c r="C47" s="107" t="s">
@@ -3139,7 +3208,7 @@
     </row>
     <row r="48" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="111" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B48" s="113"/>
       <c r="C48" s="114" t="s">
@@ -3149,7 +3218,7 @@
     </row>
     <row r="49" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="96" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B49" s="97"/>
       <c r="C49" s="98" t="s">
@@ -3159,7 +3228,7 @@
     </row>
     <row r="50" spans="1:103" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="96" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B50" s="97"/>
       <c r="C50" s="98"/>
@@ -3167,17 +3236,17 @@
     </row>
     <row r="51" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B51" s="44"/>
       <c r="C51" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D51" s="47"/>
     </row>
     <row r="52" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B52" s="44"/>
       <c r="C52" s="48" t="s">
@@ -3187,11 +3256,11 @@
     </row>
     <row r="53" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="50" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B53" s="44"/>
       <c r="C53" s="51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D53" s="74"/>
     </row>
@@ -3617,11 +3686,11 @@
       <c r="CY58" s="45"/>
     </row>
     <row r="59" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D59" s="145"/>
+      <c r="D59" s="133"/>
     </row>
     <row r="60" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="78" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B60" s="75"/>
       <c r="C60" s="76" t="s">
@@ -3679,8 +3748,8 @@
     <row r="76" spans="1:5" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.78740157480314998" bottom="0.59055118110236204" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" fitToWidth="0" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader xml:space="preserve">&amp;L&amp;G&amp;R&amp;"Times New Roman,Normal"&amp;9
 </oddHeader>
@@ -3692,25 +3761,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="A1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="87" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="87"/>
+    <col min="1" max="8" width="11.140625" style="87" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="87"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80"/>
       <c r="D1" s="82" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="83" t="s">
         <v>89</v>
-      </c>
-      <c r="F1" s="83" t="s">
-        <v>90</v>
       </c>
       <c r="G1" s="84"/>
       <c r="H1" s="85">
@@ -3723,8 +3793,7 @@
       <c r="Q1" s="85"/>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.59055118110236204" right="0.59055118110236204" top="0.98425196850393704" bottom="0.98425196850393704" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="98" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;G</oddHeader>
@@ -3736,6 +3805,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Feuil4"/>
   <dimension ref="B2:D16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3877,21 +3947,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005385EB61B379B64FA3FA00EFD5F48211" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="15b97f2a5ef9ff731d6c6b6a53c29c79">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97" xmlns:ns3="b1338d7f-541f-4bc8-84bc-74292fa164fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bdf937eed7c5c26b74985f5c8ee9608f" ns2:_="" ns3:_="">
     <xsd:import namespace="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
@@ -4056,32 +4111,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8534C3E6-3099-47F9-8B03-0EBDF0F03913}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A333848-59BB-40E8-9C6B-EB280D704CD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
-    <ds:schemaRef ds:uri="b1338d7f-541f-4bc8-84bc-74292fa164fd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8703DD9A-9B27-437E-AB91-283DE2CA9618}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4098,4 +4143,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8534C3E6-3099-47F9-8B03-0EBDF0F03913}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A333848-59BB-40E8-9C6B-EB280D704CD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
+    <ds:schemaRef ds:uri="b1338d7f-541f-4bc8-84bc-74292fa164fd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add four 3 zone dans report
</commit_message>
<xml_diff>
--- a/templates/Report Loa.xlsx
+++ b/templates/Report Loa.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D505093-01DA-46F0-BAF2-86E56118ECDA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28AA640-E70B-47AC-ACCD-21C663E3E4D3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13215" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="En-tête" sheetId="14" r:id="rId1"/>
@@ -489,9 +489,6 @@
     <t>Nombre d'essais :</t>
   </si>
   <si>
-    <t>Nombre d'eprouvette :</t>
-  </si>
-  <si>
     <t>Référence d'usinage :</t>
   </si>
   <si>
@@ -505,6 +502,9 @@
   </si>
   <si>
     <t>CONTRÔLE EFFORT</t>
+  </si>
+  <si>
+    <t>Nombre d'éprouvettes :</t>
   </si>
 </sst>
 </file>
@@ -2094,8 +2094,8 @@
   </sheetPr>
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="136" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" s="136"/>
       <c r="D3" s="136"/>
@@ -2385,7 +2385,7 @@
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="31" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="13"/>
@@ -2435,7 +2435,7 @@
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
       <c r="B33" s="30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -2445,7 +2445,7 @@
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -2455,7 +2455,7 @@
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="13"/>
@@ -2483,7 +2483,7 @@
     <row r="39" spans="1:13" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
       <c r="B39" s="40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C39" s="141"/>
       <c r="D39" s="141"/>
@@ -2577,7 +2577,7 @@
         <v>104</v>
       </c>
       <c r="C45" s="13" t="str">
-        <f>IF(AND(K45=0,L45=0),"NA",CONCATENATE(IF(K45&gt;0,"Four",""),IF(L45&gt;0,"Induction","")))</f>
+        <f>IF(AND(K45=0,L45=0),"NA",CONCATENATE(IF(K45&gt;0,"Four 3 zones à résistances",""),IF(L45&gt;0,"Induction","")))</f>
         <v>NA</v>
       </c>
       <c r="D45" s="13"/>
@@ -2739,7 +2739,7 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:CY76"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="D14" sqref="D14:D15"/>
       <selection pane="topRight" activeCell="D59" sqref="D59"/>
@@ -3945,15 +3945,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005385EB61B379B64FA3FA00EFD5F48211" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="15b97f2a5ef9ff731d6c6b6a53c29c79">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97" xmlns:ns3="b1338d7f-541f-4bc8-84bc-74292fa164fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bdf937eed7c5c26b74985f5c8ee9608f" ns2:_="" ns3:_="">
     <xsd:import namespace="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
@@ -4118,6 +4109,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4125,14 +4125,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8534C3E6-3099-47F9-8B03-0EBDF0F03913}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8703DD9A-9B27-437E-AB91-283DE2CA9618}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4147,6 +4139,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8534C3E6-3099-47F9-8B03-0EBDF0F03913}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
add void dans report + suppression OLD
</commit_message>
<xml_diff>
--- a/templates/Report Loa.xlsx
+++ b/templates/Report Loa.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7103F477-8F6A-4AB7-A73A-44BA1881E878}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4AE694-7714-4C58-B0D7-BFAEED204692}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13215" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="En-tête" sheetId="14" r:id="rId1"/>
@@ -1206,8 +1206,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1495,6 +1493,12 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2094,7 +2098,7 @@
   </sheetPr>
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
@@ -2114,32 +2118,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="137"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="135"/>
     </row>
     <row r="2" spans="1:8" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="133" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="137"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="135"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="136" t="s">
+      <c r="B3" s="134" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
-      <c r="F3" s="136"/>
-      <c r="G3" s="137"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="135"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" s="17"/>
@@ -2147,7 +2151,7 @@
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
-      <c r="G4" s="137"/>
+      <c r="G4" s="135"/>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
@@ -2160,7 +2164,7 @@
         <v>98</v>
       </c>
       <c r="F5" s="19"/>
-      <c r="G5" s="137"/>
+      <c r="G5" s="135"/>
     </row>
     <row r="6" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="18"/>
@@ -2172,7 +2176,7 @@
       <c r="F6" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="137"/>
+      <c r="G6" s="135"/>
     </row>
     <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="18"/>
@@ -2182,7 +2186,7 @@
         <v>97</v>
       </c>
       <c r="F7" s="20"/>
-      <c r="G7" s="137"/>
+      <c r="G7" s="135"/>
     </row>
     <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="18"/>
@@ -2190,7 +2194,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="25"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="137"/>
+      <c r="G8" s="135"/>
     </row>
     <row r="9" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="18"/>
@@ -2200,7 +2204,7 @@
         <v>113</v>
       </c>
       <c r="F9" s="20"/>
-      <c r="G9" s="137"/>
+      <c r="G9" s="135"/>
     </row>
     <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="21"/>
@@ -2208,7 +2212,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="26"/>
       <c r="F10" s="22"/>
-      <c r="G10" s="137"/>
+      <c r="G10" s="135"/>
     </row>
     <row r="11" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="18"/>
@@ -2216,7 +2220,7 @@
       <c r="D11" s="17"/>
       <c r="E11" s="25"/>
       <c r="F11" s="23"/>
-      <c r="G11" s="137"/>
+      <c r="G11" s="135"/>
     </row>
     <row r="12" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="18"/>
@@ -2233,57 +2237,57 @@
       <c r="B13" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="142" t="s">
+      <c r="C13" s="140" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="143"/>
-      <c r="E13" s="143"/>
-      <c r="F13" s="143"/>
-      <c r="G13" s="143"/>
-      <c r="H13" s="144"/>
+      <c r="D13" s="141"/>
+      <c r="E13" s="141"/>
+      <c r="F13" s="141"/>
+      <c r="G13" s="141"/>
+      <c r="H13" s="142"/>
     </row>
     <row r="14" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="35"/>
       <c r="B14" s="36"/>
-      <c r="C14" s="145"/>
-      <c r="D14" s="145"/>
-      <c r="E14" s="145"/>
-      <c r="F14" s="145"/>
-      <c r="G14" s="145"/>
-      <c r="H14" s="145"/>
+      <c r="C14" s="143"/>
+      <c r="D14" s="143"/>
+      <c r="E14" s="143"/>
+      <c r="F14" s="143"/>
+      <c r="G14" s="143"/>
+      <c r="H14" s="143"/>
     </row>
     <row r="15" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="37"/>
       <c r="B15" s="38"/>
-      <c r="C15" s="146"/>
-      <c r="D15" s="146"/>
-      <c r="E15" s="146"/>
-      <c r="F15" s="146"/>
-      <c r="G15" s="146"/>
-      <c r="H15" s="146"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="144"/>
+      <c r="F15" s="144"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="144"/>
     </row>
     <row r="16" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="39"/>
       <c r="B16" s="38"/>
-      <c r="C16" s="147"/>
-      <c r="D16" s="147"/>
-      <c r="E16" s="147"/>
-      <c r="F16" s="147"/>
-      <c r="G16" s="147"/>
-      <c r="H16" s="147"/>
+      <c r="C16" s="145"/>
+      <c r="D16" s="145"/>
+      <c r="E16" s="145"/>
+      <c r="F16" s="145"/>
+      <c r="G16" s="145"/>
+      <c r="H16" s="145"/>
     </row>
     <row r="17" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="140" t="s">
+      <c r="A18" s="138" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="140"/>
-      <c r="C18" s="140"/>
-      <c r="D18" s="140"/>
-      <c r="E18" s="140"/>
-      <c r="F18" s="140"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="140"/>
+      <c r="B18" s="138"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
+      <c r="F18" s="138"/>
+      <c r="G18" s="138"/>
+      <c r="H18" s="138"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
@@ -2296,21 +2300,21 @@
       <c r="B20" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="148"/>
-      <c r="D20" s="148"/>
-      <c r="E20" s="148"/>
-      <c r="F20" s="148"/>
-      <c r="G20" s="148"/>
-      <c r="H20" s="148"/>
+      <c r="C20" s="146"/>
+      <c r="D20" s="146"/>
+      <c r="E20" s="146"/>
+      <c r="F20" s="146"/>
+      <c r="G20" s="146"/>
+      <c r="H20" s="146"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="C21" s="148"/>
-      <c r="D21" s="148"/>
-      <c r="E21" s="148"/>
-      <c r="F21" s="148"/>
-      <c r="G21" s="148"/>
-      <c r="H21" s="148"/>
+      <c r="C21" s="146"/>
+      <c r="D21" s="146"/>
+      <c r="E21" s="146"/>
+      <c r="F21" s="146"/>
+      <c r="G21" s="146"/>
+      <c r="H21" s="146"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
@@ -2409,7 +2413,7 @@
       <c r="D31" s="13"/>
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
-      <c r="M31" s="90"/>
+      <c r="M31" s="88"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
@@ -2423,14 +2427,14 @@
       <c r="D32" s="13"/>
       <c r="E32" s="33"/>
       <c r="F32" s="16"/>
-      <c r="K32" s="91"/>
-      <c r="L32" s="92" t="s">
+      <c r="K32" s="89"/>
+      <c r="L32" s="90" t="s">
         <v>112</v>
       </c>
-      <c r="M32" s="93" t="s">
+      <c r="M32" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="N32" s="91"/>
+      <c r="N32" s="89"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
@@ -2466,16 +2470,16 @@
       <c r="A36" s="5"/>
     </row>
     <row r="37" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="140" t="s">
+      <c r="A37" s="138" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="140"/>
-      <c r="C37" s="140"/>
-      <c r="D37" s="140"/>
-      <c r="E37" s="140"/>
-      <c r="F37" s="140"/>
-      <c r="G37" s="140"/>
-      <c r="H37" s="140"/>
+      <c r="B37" s="138"/>
+      <c r="C37" s="138"/>
+      <c r="D37" s="138"/>
+      <c r="E37" s="138"/>
+      <c r="F37" s="138"/>
+      <c r="G37" s="138"/>
+      <c r="H37" s="138"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
@@ -2485,11 +2489,11 @@
       <c r="B39" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="C39" s="141"/>
-      <c r="D39" s="141"/>
-      <c r="E39" s="141"/>
-      <c r="F39" s="141"/>
-      <c r="G39" s="141"/>
+      <c r="C39" s="139"/>
+      <c r="D39" s="139"/>
+      <c r="E39" s="139"/>
+      <c r="F39" s="139"/>
+      <c r="G39" s="139"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
@@ -2499,9 +2503,9 @@
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
       <c r="G40" s="15"/>
-      <c r="K40" s="88"/>
-      <c r="L40" s="88"/>
-      <c r="M40" s="88"/>
+      <c r="K40" s="86"/>
+      <c r="L40" s="86"/>
+      <c r="M40" s="86"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
@@ -2515,9 +2519,9 @@
       <c r="E41" s="13"/>
       <c r="F41" s="13"/>
       <c r="G41" s="15"/>
-      <c r="K41" s="88"/>
-      <c r="L41" s="88"/>
-      <c r="M41" s="88"/>
+      <c r="K41" s="86"/>
+      <c r="L41" s="86"/>
+      <c r="M41" s="86"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
@@ -2533,43 +2537,43 @@
       </c>
       <c r="F42" s="13"/>
       <c r="G42" s="15"/>
-      <c r="K42" s="88"/>
-      <c r="L42" s="88"/>
-      <c r="M42" s="88"/>
+      <c r="K42" s="86"/>
+      <c r="L42" s="86"/>
+      <c r="M42" s="86"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
       <c r="B43" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="139" t="str">
+      <c r="C43" s="137" t="str">
         <f>CONCATENATE("Système hydraulique de ",K43," kN avec servovalve contrôlé par une boucle d'asservissement.")</f>
         <v>Système hydraulique de xxx kN avec servovalve contrôlé par une boucle d'asservissement.</v>
       </c>
-      <c r="D43" s="139"/>
-      <c r="E43" s="139"/>
-      <c r="F43" s="139"/>
-      <c r="G43" s="139"/>
-      <c r="H43" s="139"/>
-      <c r="K43" s="91" t="s">
+      <c r="D43" s="137"/>
+      <c r="E43" s="137"/>
+      <c r="F43" s="137"/>
+      <c r="G43" s="137"/>
+      <c r="H43" s="137"/>
+      <c r="K43" s="89" t="s">
         <v>90</v>
       </c>
-      <c r="L43" s="88"/>
-      <c r="M43" s="88"/>
+      <c r="L43" s="86"/>
+      <c r="M43" s="86"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
       <c r="B44" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="89"/>
+      <c r="C44" s="87"/>
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
       <c r="G44" s="15"/>
-      <c r="K44" s="88"/>
-      <c r="L44" s="88"/>
-      <c r="M44" s="88"/>
+      <c r="K44" s="86"/>
+      <c r="L44" s="86"/>
+      <c r="M44" s="86"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
@@ -2584,9 +2588,9 @@
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
       <c r="G45" s="15"/>
-      <c r="K45" s="88"/>
-      <c r="L45" s="88"/>
-      <c r="M45" s="88"/>
+      <c r="K45" s="86"/>
+      <c r="L45" s="86"/>
+      <c r="M45" s="86"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
@@ -2596,9 +2600,9 @@
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
-      <c r="K46" s="88"/>
-      <c r="L46" s="88"/>
-      <c r="M46" s="88"/>
+      <c r="K46" s="86"/>
+      <c r="L46" s="86"/>
+      <c r="M46" s="86"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
@@ -2608,9 +2612,9 @@
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
       <c r="G47" s="15"/>
-      <c r="K47" s="88"/>
-      <c r="L47" s="88"/>
-      <c r="M47" s="88"/>
+      <c r="K47" s="86"/>
+      <c r="L47" s="86"/>
+      <c r="M47" s="86"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="5"/>
@@ -2620,9 +2624,9 @@
       <c r="E48" s="16"/>
       <c r="F48" s="16"/>
       <c r="G48" s="12"/>
-      <c r="K48" s="88"/>
-      <c r="L48" s="88"/>
-      <c r="M48" s="88"/>
+      <c r="K48" s="86"/>
+      <c r="L48" s="86"/>
+      <c r="M48" s="86"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
@@ -2636,9 +2640,9 @@
         <v>37</v>
       </c>
       <c r="G49" s="5"/>
-      <c r="K49" s="88"/>
-      <c r="L49" s="88"/>
-      <c r="M49" s="88"/>
+      <c r="K49" s="86"/>
+      <c r="L49" s="86"/>
+      <c r="M49" s="86"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
@@ -2675,8 +2679,8 @@
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
-      <c r="G52" s="138"/>
-      <c r="H52" s="138"/>
+      <c r="G52" s="136"/>
+      <c r="H52" s="136"/>
       <c r="K52" s="6"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
@@ -2688,8 +2692,8 @@
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
-      <c r="G53" s="138"/>
-      <c r="H53" s="138"/>
+      <c r="G53" s="136"/>
+      <c r="H53" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2739,10 +2743,10 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:CY76"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="D14" sqref="D14:D15"/>
-      <selection pane="topRight" activeCell="D59" sqref="D59"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2753,995 +2757,995 @@
     <col min="4" max="87" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="94" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P1" s="95" t="s">
+    <row r="1" spans="1:16" s="92" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P1" s="93" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="41" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="42"/>
+    <row r="4" spans="1:16" s="147" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="148"/>
     </row>
     <row r="5" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="98" t="s">
+      <c r="B5" s="95"/>
+      <c r="C5" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="99"/>
+      <c r="D5" s="97"/>
     </row>
     <row r="6" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="98" t="s">
+      <c r="B6" s="95"/>
+      <c r="C6" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="99"/>
+      <c r="D6" s="97"/>
     </row>
     <row r="7" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="46" t="s">
+      <c r="B7" s="42"/>
+      <c r="C7" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="47"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="48" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="47"/>
+      <c r="D8" s="45"/>
     </row>
     <row r="9" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="48" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="47"/>
+      <c r="D9" s="45"/>
     </row>
     <row r="10" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="47"/>
     </row>
     <row r="11" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="51" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="45"/>
     </row>
     <row r="12" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="51" t="s">
+      <c r="B12" s="42"/>
+      <c r="C12" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="47"/>
+      <c r="D12" s="45"/>
     </row>
     <row r="13" spans="1:16" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="51" t="s">
+      <c r="B13" s="42"/>
+      <c r="C13" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="47"/>
+      <c r="D13" s="45"/>
     </row>
     <row r="14" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="105"/>
-      <c r="B14" s="106" t="s">
+      <c r="A14" s="103"/>
+      <c r="B14" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="107" t="s">
+      <c r="C14" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="108"/>
+      <c r="D14" s="106"/>
     </row>
     <row r="15" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="105"/>
-      <c r="B15" s="106" t="s">
+      <c r="A15" s="103"/>
+      <c r="B15" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="107" t="s">
+      <c r="C15" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="117"/>
+      <c r="D15" s="115"/>
     </row>
     <row r="16" spans="1:16" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="111" t="s">
+      <c r="A16" s="109" t="s">
         <v>116</v>
       </c>
-      <c r="B16" s="106"/>
-      <c r="C16" s="107" t="s">
+      <c r="B16" s="104"/>
+      <c r="C16" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="118"/>
+      <c r="D16" s="116"/>
     </row>
     <row r="17" spans="1:4" ht="14.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="128" t="s">
+      <c r="A17" s="126" t="s">
         <v>117</v>
       </c>
-      <c r="B17" s="109"/>
-      <c r="C17" s="127" t="str">
+      <c r="B17" s="107"/>
+      <c r="C17" s="125" t="str">
         <f>IF(C14="",C15,C14)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D17" s="110"/>
+      <c r="D17" s="108"/>
     </row>
     <row r="18" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54" t="s">
+      <c r="B18" s="51"/>
+      <c r="C18" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="55"/>
+      <c r="D18" s="53"/>
     </row>
     <row r="19" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="51" t="s">
+      <c r="B19" s="42"/>
+      <c r="C19" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="56"/>
+      <c r="D19" s="54"/>
     </row>
     <row r="20" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="51" t="s">
+      <c r="B20" s="42"/>
+      <c r="C20" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="56"/>
+      <c r="D20" s="54"/>
     </row>
     <row r="21" spans="1:4" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="58"/>
-      <c r="C21" s="59" t="s">
+      <c r="B21" s="56"/>
+      <c r="C21" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="60"/>
+      <c r="D21" s="58"/>
     </row>
     <row r="22" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="119" t="s">
+      <c r="A22" s="117" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="120"/>
-      <c r="C22" s="121" t="s">
+      <c r="B22" s="118"/>
+      <c r="C22" s="119" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="122"/>
+      <c r="D22" s="120"/>
     </row>
     <row r="23" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="61" t="s">
+      <c r="A23" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="62"/>
-      <c r="C23" s="51" t="s">
+      <c r="B23" s="60"/>
+      <c r="C23" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="63"/>
+      <c r="D23" s="61"/>
     </row>
     <row r="24" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="63"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="61"/>
     </row>
     <row r="25" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="61" t="s">
+      <c r="A25" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="51" t="s">
+      <c r="B25" s="62"/>
+      <c r="C25" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="63"/>
+      <c r="D25" s="61"/>
     </row>
     <row r="26" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="62"/>
-      <c r="C26" s="51" t="s">
+      <c r="B26" s="60"/>
+      <c r="C26" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="65"/>
+      <c r="D26" s="63"/>
     </row>
     <row r="27" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="61" t="s">
+      <c r="A27" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="64"/>
-      <c r="C27" s="51" t="s">
+      <c r="B27" s="62"/>
+      <c r="C27" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="66"/>
+      <c r="D27" s="64"/>
     </row>
     <row r="28" spans="1:4" ht="14.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="58"/>
-      <c r="C28" s="59" t="s">
+      <c r="B28" s="56"/>
+      <c r="C28" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="123"/>
+      <c r="D28" s="121"/>
     </row>
     <row r="29" spans="1:4" ht="14.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="129" t="s">
+      <c r="A29" s="127" t="s">
         <v>118</v>
       </c>
-      <c r="B29" s="130"/>
-      <c r="C29" s="131"/>
-      <c r="D29" s="132"/>
+      <c r="B29" s="128"/>
+      <c r="C29" s="129"/>
+      <c r="D29" s="130"/>
     </row>
     <row r="30" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="124" t="s">
+      <c r="A30" s="122" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="125" t="s">
+      <c r="B30" s="123" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="54" t="s">
+      <c r="C30" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="126"/>
+      <c r="D30" s="124"/>
     </row>
     <row r="31" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="61" t="s">
+      <c r="A31" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="67" t="s">
+      <c r="B31" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="63"/>
+      <c r="D31" s="61"/>
     </row>
     <row r="32" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="61" t="s">
+      <c r="A32" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="67" t="s">
+      <c r="B32" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="51" t="s">
+      <c r="C32" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="63"/>
+      <c r="D32" s="61"/>
     </row>
     <row r="33" spans="1:4" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="68" t="s">
+      <c r="A33" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="69" t="s">
+      <c r="B33" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="59" t="s">
+      <c r="C33" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="70"/>
+      <c r="D33" s="68"/>
     </row>
     <row r="34" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="52" t="s">
+      <c r="A34" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="53"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="55"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="53"/>
     </row>
     <row r="35" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="61" t="s">
+      <c r="A35" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="62" t="s">
+      <c r="B35" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="51" t="s">
+      <c r="C35" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="63"/>
+      <c r="D35" s="61"/>
     </row>
     <row r="36" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="61" t="s">
+      <c r="A36" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="64" t="s">
+      <c r="B36" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="51" t="s">
+      <c r="C36" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="63"/>
+      <c r="D36" s="61"/>
     </row>
     <row r="37" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="61" t="s">
+      <c r="A37" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="64" t="s">
+      <c r="B37" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="51" t="s">
+      <c r="C37" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="D37" s="63"/>
+      <c r="D37" s="61"/>
     </row>
     <row r="38" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="43" t="s">
+      <c r="A38" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="62" t="s">
+      <c r="B38" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="51" t="s">
+      <c r="C38" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="65"/>
+      <c r="D38" s="63"/>
     </row>
     <row r="39" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="61" t="s">
+      <c r="A39" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="64" t="s">
+      <c r="B39" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="51" t="s">
+      <c r="C39" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="66"/>
+      <c r="D39" s="64"/>
     </row>
     <row r="40" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="61" t="s">
+      <c r="A40" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="64" t="s">
+      <c r="B40" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="51" t="s">
+      <c r="C40" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="71"/>
+      <c r="D40" s="69"/>
     </row>
     <row r="41" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="61" t="s">
+      <c r="A41" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="64" t="s">
+      <c r="B41" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="51" t="s">
+      <c r="C41" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="71"/>
+      <c r="D41" s="69"/>
     </row>
     <row r="42" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="61" t="s">
+      <c r="A42" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="64" t="s">
+      <c r="B42" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="51" t="s">
+      <c r="C42" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="71"/>
+      <c r="D42" s="69"/>
     </row>
     <row r="43" spans="1:4" ht="14.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="68" t="s">
+      <c r="A43" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="58" t="s">
+      <c r="B43" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="59" t="s">
+      <c r="C43" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="72"/>
+      <c r="D43" s="70"/>
     </row>
     <row r="44" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="52" t="s">
+      <c r="A44" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="53"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="55"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="53"/>
     </row>
     <row r="45" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="43" t="s">
+      <c r="A45" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="44"/>
-      <c r="C45" s="48"/>
-      <c r="D45" s="47"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="45"/>
     </row>
     <row r="46" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="44"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="47"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="45"/>
     </row>
     <row r="47" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="111" t="s">
+      <c r="A47" s="109" t="s">
         <v>94</v>
       </c>
-      <c r="B47" s="106"/>
-      <c r="C47" s="107" t="s">
+      <c r="B47" s="104"/>
+      <c r="C47" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="112"/>
+      <c r="D47" s="110"/>
     </row>
     <row r="48" spans="1:4" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="111" t="s">
+      <c r="A48" s="109" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="113"/>
-      <c r="C48" s="114" t="s">
+      <c r="B48" s="111"/>
+      <c r="C48" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="D48" s="115"/>
+      <c r="D48" s="113"/>
     </row>
     <row r="49" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="96" t="s">
+      <c r="A49" s="94" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="97"/>
-      <c r="C49" s="98" t="s">
+      <c r="B49" s="95"/>
+      <c r="C49" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="D49" s="116"/>
+      <c r="D49" s="114"/>
     </row>
     <row r="50" spans="1:103" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="96" t="s">
+      <c r="A50" s="94" t="s">
         <v>119</v>
       </c>
-      <c r="B50" s="97"/>
-      <c r="C50" s="98"/>
-      <c r="D50" s="116"/>
+      <c r="B50" s="95"/>
+      <c r="C50" s="96"/>
+      <c r="D50" s="114"/>
     </row>
     <row r="51" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="50" t="s">
+      <c r="A51" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="B51" s="44"/>
-      <c r="C51" s="51" t="s">
+      <c r="B51" s="42"/>
+      <c r="C51" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="D51" s="47"/>
+      <c r="D51" s="45"/>
     </row>
     <row r="52" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="43" t="s">
+      <c r="A52" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="44"/>
-      <c r="C52" s="48" t="s">
+      <c r="B52" s="42"/>
+      <c r="C52" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D52" s="73"/>
+      <c r="D52" s="71"/>
     </row>
     <row r="53" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="50" t="s">
+      <c r="A53" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="44"/>
-      <c r="C53" s="51" t="s">
+      <c r="B53" s="42"/>
+      <c r="C53" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="D53" s="74"/>
-    </row>
-    <row r="54" spans="1:103" s="104" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="101"/>
-      <c r="B54" s="102"/>
-      <c r="C54" s="103"/>
+      <c r="D53" s="72"/>
+    </row>
+    <row r="54" spans="1:103" s="102" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="99"/>
+      <c r="B54" s="100"/>
+      <c r="C54" s="101"/>
     </row>
     <row r="55" spans="1:103" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="45" t="s">
+      <c r="A55" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B55" s="75"/>
-      <c r="C55" s="45" t="s">
+      <c r="B55" s="73"/>
+      <c r="C55" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="F55" s="45"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="45"/>
-      <c r="J55" s="45"/>
-      <c r="K55" s="45"/>
-      <c r="L55" s="45"/>
-      <c r="M55" s="45"/>
-      <c r="N55" s="45"/>
-      <c r="O55" s="45"/>
-      <c r="P55" s="45"/>
-      <c r="Q55" s="45"/>
-      <c r="R55" s="45"/>
-      <c r="S55" s="45"/>
-      <c r="T55" s="45"/>
-      <c r="U55" s="45"/>
-      <c r="V55" s="45"/>
-      <c r="W55" s="45"/>
-      <c r="X55" s="45"/>
-      <c r="Y55" s="45"/>
-      <c r="Z55" s="45"/>
-      <c r="AA55" s="45"/>
-      <c r="AB55" s="45"/>
-      <c r="AC55" s="45"/>
-      <c r="AD55" s="45"/>
-      <c r="AE55" s="45"/>
-      <c r="AF55" s="45"/>
-      <c r="AG55" s="45"/>
-      <c r="AH55" s="45"/>
-      <c r="AI55" s="45"/>
-      <c r="AJ55" s="45"/>
-      <c r="AK55" s="45"/>
-      <c r="AL55" s="45"/>
-      <c r="AM55" s="45"/>
-      <c r="AN55" s="45"/>
-      <c r="AO55" s="45"/>
-      <c r="AP55" s="45"/>
-      <c r="AQ55" s="45"/>
-      <c r="AR55" s="45"/>
-      <c r="AS55" s="45"/>
-      <c r="AT55" s="45"/>
-      <c r="AU55" s="45"/>
-      <c r="AV55" s="45"/>
-      <c r="AW55" s="45"/>
-      <c r="AX55" s="45"/>
-      <c r="AY55" s="45"/>
-      <c r="AZ55" s="45"/>
-      <c r="BA55" s="45"/>
-      <c r="BB55" s="45"/>
-      <c r="BC55" s="45"/>
-      <c r="BD55" s="45"/>
-      <c r="BE55" s="45"/>
-      <c r="BF55" s="45"/>
-      <c r="BG55" s="45"/>
-      <c r="BH55" s="45"/>
-      <c r="BI55" s="45"/>
-      <c r="BJ55" s="45"/>
-      <c r="BK55" s="45"/>
-      <c r="BL55" s="45"/>
-      <c r="BM55" s="45"/>
-      <c r="BN55" s="45"/>
-      <c r="BO55" s="45"/>
-      <c r="BP55" s="45"/>
-      <c r="BQ55" s="45"/>
-      <c r="BR55" s="45"/>
-      <c r="BS55" s="45"/>
-      <c r="BT55" s="45"/>
-      <c r="BU55" s="45"/>
-      <c r="BV55" s="45"/>
-      <c r="BW55" s="45"/>
-      <c r="BX55" s="45"/>
-      <c r="BY55" s="45"/>
-      <c r="BZ55" s="45"/>
-      <c r="CA55" s="45"/>
-      <c r="CB55" s="45"/>
-      <c r="CC55" s="45"/>
-      <c r="CD55" s="45"/>
-      <c r="CE55" s="45"/>
-      <c r="CF55" s="45"/>
-      <c r="CG55" s="45"/>
-      <c r="CH55" s="45"/>
-      <c r="CI55" s="45"/>
-      <c r="CJ55" s="45"/>
-      <c r="CK55" s="45"/>
-      <c r="CL55" s="45"/>
-      <c r="CM55" s="45"/>
-      <c r="CN55" s="45"/>
-      <c r="CO55" s="45"/>
-      <c r="CP55" s="45"/>
-      <c r="CQ55" s="45"/>
-      <c r="CR55" s="45"/>
-      <c r="CS55" s="45"/>
-      <c r="CT55" s="45"/>
-      <c r="CU55" s="45"/>
-      <c r="CV55" s="45"/>
-      <c r="CW55" s="45"/>
-      <c r="CX55" s="45"/>
-      <c r="CY55" s="45"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="43"/>
+      <c r="I55" s="43"/>
+      <c r="J55" s="43"/>
+      <c r="K55" s="43"/>
+      <c r="L55" s="43"/>
+      <c r="M55" s="43"/>
+      <c r="N55" s="43"/>
+      <c r="O55" s="43"/>
+      <c r="P55" s="43"/>
+      <c r="Q55" s="43"/>
+      <c r="R55" s="43"/>
+      <c r="S55" s="43"/>
+      <c r="T55" s="43"/>
+      <c r="U55" s="43"/>
+      <c r="V55" s="43"/>
+      <c r="W55" s="43"/>
+      <c r="X55" s="43"/>
+      <c r="Y55" s="43"/>
+      <c r="Z55" s="43"/>
+      <c r="AA55" s="43"/>
+      <c r="AB55" s="43"/>
+      <c r="AC55" s="43"/>
+      <c r="AD55" s="43"/>
+      <c r="AE55" s="43"/>
+      <c r="AF55" s="43"/>
+      <c r="AG55" s="43"/>
+      <c r="AH55" s="43"/>
+      <c r="AI55" s="43"/>
+      <c r="AJ55" s="43"/>
+      <c r="AK55" s="43"/>
+      <c r="AL55" s="43"/>
+      <c r="AM55" s="43"/>
+      <c r="AN55" s="43"/>
+      <c r="AO55" s="43"/>
+      <c r="AP55" s="43"/>
+      <c r="AQ55" s="43"/>
+      <c r="AR55" s="43"/>
+      <c r="AS55" s="43"/>
+      <c r="AT55" s="43"/>
+      <c r="AU55" s="43"/>
+      <c r="AV55" s="43"/>
+      <c r="AW55" s="43"/>
+      <c r="AX55" s="43"/>
+      <c r="AY55" s="43"/>
+      <c r="AZ55" s="43"/>
+      <c r="BA55" s="43"/>
+      <c r="BB55" s="43"/>
+      <c r="BC55" s="43"/>
+      <c r="BD55" s="43"/>
+      <c r="BE55" s="43"/>
+      <c r="BF55" s="43"/>
+      <c r="BG55" s="43"/>
+      <c r="BH55" s="43"/>
+      <c r="BI55" s="43"/>
+      <c r="BJ55" s="43"/>
+      <c r="BK55" s="43"/>
+      <c r="BL55" s="43"/>
+      <c r="BM55" s="43"/>
+      <c r="BN55" s="43"/>
+      <c r="BO55" s="43"/>
+      <c r="BP55" s="43"/>
+      <c r="BQ55" s="43"/>
+      <c r="BR55" s="43"/>
+      <c r="BS55" s="43"/>
+      <c r="BT55" s="43"/>
+      <c r="BU55" s="43"/>
+      <c r="BV55" s="43"/>
+      <c r="BW55" s="43"/>
+      <c r="BX55" s="43"/>
+      <c r="BY55" s="43"/>
+      <c r="BZ55" s="43"/>
+      <c r="CA55" s="43"/>
+      <c r="CB55" s="43"/>
+      <c r="CC55" s="43"/>
+      <c r="CD55" s="43"/>
+      <c r="CE55" s="43"/>
+      <c r="CF55" s="43"/>
+      <c r="CG55" s="43"/>
+      <c r="CH55" s="43"/>
+      <c r="CI55" s="43"/>
+      <c r="CJ55" s="43"/>
+      <c r="CK55" s="43"/>
+      <c r="CL55" s="43"/>
+      <c r="CM55" s="43"/>
+      <c r="CN55" s="43"/>
+      <c r="CO55" s="43"/>
+      <c r="CP55" s="43"/>
+      <c r="CQ55" s="43"/>
+      <c r="CR55" s="43"/>
+      <c r="CS55" s="43"/>
+      <c r="CT55" s="43"/>
+      <c r="CU55" s="43"/>
+      <c r="CV55" s="43"/>
+      <c r="CW55" s="43"/>
+      <c r="CX55" s="43"/>
+      <c r="CY55" s="43"/>
     </row>
     <row r="56" spans="1:103" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="45"/>
-      <c r="B56" s="75"/>
-      <c r="C56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="45"/>
-      <c r="J56" s="45"/>
-      <c r="K56" s="45"/>
-      <c r="L56" s="45"/>
-      <c r="M56" s="45"/>
-      <c r="N56" s="45"/>
-      <c r="O56" s="45"/>
-      <c r="P56" s="45"/>
-      <c r="Q56" s="45"/>
-      <c r="R56" s="45"/>
-      <c r="S56" s="45"/>
-      <c r="T56" s="45"/>
-      <c r="U56" s="45"/>
-      <c r="V56" s="45"/>
-      <c r="W56" s="45"/>
-      <c r="X56" s="45"/>
-      <c r="Y56" s="45"/>
-      <c r="Z56" s="45"/>
-      <c r="AA56" s="45"/>
-      <c r="AB56" s="45"/>
-      <c r="AC56" s="45"/>
-      <c r="AD56" s="45"/>
-      <c r="AE56" s="45"/>
-      <c r="AF56" s="45"/>
-      <c r="AG56" s="45"/>
-      <c r="AH56" s="45"/>
-      <c r="AI56" s="45"/>
-      <c r="AJ56" s="45"/>
-      <c r="AK56" s="45"/>
-      <c r="AL56" s="45"/>
-      <c r="AM56" s="45"/>
-      <c r="AN56" s="45"/>
-      <c r="AO56" s="45"/>
-      <c r="AP56" s="45"/>
-      <c r="AQ56" s="45"/>
-      <c r="AR56" s="45"/>
-      <c r="AS56" s="45"/>
-      <c r="AT56" s="45"/>
-      <c r="AU56" s="45"/>
-      <c r="AV56" s="45"/>
-      <c r="AW56" s="45"/>
-      <c r="AX56" s="45"/>
-      <c r="AY56" s="45"/>
-      <c r="AZ56" s="45"/>
-      <c r="BA56" s="45"/>
-      <c r="BB56" s="45"/>
-      <c r="BC56" s="45"/>
-      <c r="BD56" s="45"/>
-      <c r="BE56" s="45"/>
-      <c r="BF56" s="45"/>
-      <c r="BG56" s="45"/>
-      <c r="BH56" s="45"/>
-      <c r="BI56" s="45"/>
-      <c r="BJ56" s="45"/>
-      <c r="BK56" s="45"/>
-      <c r="BL56" s="45"/>
-      <c r="BM56" s="45"/>
-      <c r="BN56" s="45"/>
-      <c r="BO56" s="45"/>
-      <c r="BP56" s="45"/>
-      <c r="BQ56" s="45"/>
-      <c r="BR56" s="45"/>
-      <c r="BS56" s="45"/>
-      <c r="BT56" s="45"/>
-      <c r="BU56" s="45"/>
-      <c r="BV56" s="45"/>
-      <c r="BW56" s="45"/>
-      <c r="BX56" s="45"/>
-      <c r="BY56" s="45"/>
-      <c r="BZ56" s="45"/>
-      <c r="CA56" s="45"/>
-      <c r="CB56" s="45"/>
-      <c r="CC56" s="45"/>
-      <c r="CD56" s="45"/>
-      <c r="CE56" s="45"/>
-      <c r="CF56" s="45"/>
-      <c r="CG56" s="45"/>
-      <c r="CH56" s="45"/>
-      <c r="CI56" s="45"/>
-      <c r="CJ56" s="45"/>
-      <c r="CK56" s="45"/>
-      <c r="CL56" s="45"/>
-      <c r="CM56" s="45"/>
-      <c r="CN56" s="45"/>
-      <c r="CO56" s="45"/>
-      <c r="CP56" s="45"/>
-      <c r="CQ56" s="45"/>
-      <c r="CR56" s="45"/>
-      <c r="CS56" s="45"/>
-      <c r="CT56" s="45"/>
-      <c r="CU56" s="45"/>
-      <c r="CV56" s="45"/>
-      <c r="CW56" s="45"/>
-      <c r="CX56" s="45"/>
-      <c r="CY56" s="45"/>
+      <c r="A56" s="43"/>
+      <c r="B56" s="73"/>
+      <c r="C56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="43"/>
+      <c r="J56" s="43"/>
+      <c r="K56" s="43"/>
+      <c r="L56" s="43"/>
+      <c r="M56" s="43"/>
+      <c r="N56" s="43"/>
+      <c r="O56" s="43"/>
+      <c r="P56" s="43"/>
+      <c r="Q56" s="43"/>
+      <c r="R56" s="43"/>
+      <c r="S56" s="43"/>
+      <c r="T56" s="43"/>
+      <c r="U56" s="43"/>
+      <c r="V56" s="43"/>
+      <c r="W56" s="43"/>
+      <c r="X56" s="43"/>
+      <c r="Y56" s="43"/>
+      <c r="Z56" s="43"/>
+      <c r="AA56" s="43"/>
+      <c r="AB56" s="43"/>
+      <c r="AC56" s="43"/>
+      <c r="AD56" s="43"/>
+      <c r="AE56" s="43"/>
+      <c r="AF56" s="43"/>
+      <c r="AG56" s="43"/>
+      <c r="AH56" s="43"/>
+      <c r="AI56" s="43"/>
+      <c r="AJ56" s="43"/>
+      <c r="AK56" s="43"/>
+      <c r="AL56" s="43"/>
+      <c r="AM56" s="43"/>
+      <c r="AN56" s="43"/>
+      <c r="AO56" s="43"/>
+      <c r="AP56" s="43"/>
+      <c r="AQ56" s="43"/>
+      <c r="AR56" s="43"/>
+      <c r="AS56" s="43"/>
+      <c r="AT56" s="43"/>
+      <c r="AU56" s="43"/>
+      <c r="AV56" s="43"/>
+      <c r="AW56" s="43"/>
+      <c r="AX56" s="43"/>
+      <c r="AY56" s="43"/>
+      <c r="AZ56" s="43"/>
+      <c r="BA56" s="43"/>
+      <c r="BB56" s="43"/>
+      <c r="BC56" s="43"/>
+      <c r="BD56" s="43"/>
+      <c r="BE56" s="43"/>
+      <c r="BF56" s="43"/>
+      <c r="BG56" s="43"/>
+      <c r="BH56" s="43"/>
+      <c r="BI56" s="43"/>
+      <c r="BJ56" s="43"/>
+      <c r="BK56" s="43"/>
+      <c r="BL56" s="43"/>
+      <c r="BM56" s="43"/>
+      <c r="BN56" s="43"/>
+      <c r="BO56" s="43"/>
+      <c r="BP56" s="43"/>
+      <c r="BQ56" s="43"/>
+      <c r="BR56" s="43"/>
+      <c r="BS56" s="43"/>
+      <c r="BT56" s="43"/>
+      <c r="BU56" s="43"/>
+      <c r="BV56" s="43"/>
+      <c r="BW56" s="43"/>
+      <c r="BX56" s="43"/>
+      <c r="BY56" s="43"/>
+      <c r="BZ56" s="43"/>
+      <c r="CA56" s="43"/>
+      <c r="CB56" s="43"/>
+      <c r="CC56" s="43"/>
+      <c r="CD56" s="43"/>
+      <c r="CE56" s="43"/>
+      <c r="CF56" s="43"/>
+      <c r="CG56" s="43"/>
+      <c r="CH56" s="43"/>
+      <c r="CI56" s="43"/>
+      <c r="CJ56" s="43"/>
+      <c r="CK56" s="43"/>
+      <c r="CL56" s="43"/>
+      <c r="CM56" s="43"/>
+      <c r="CN56" s="43"/>
+      <c r="CO56" s="43"/>
+      <c r="CP56" s="43"/>
+      <c r="CQ56" s="43"/>
+      <c r="CR56" s="43"/>
+      <c r="CS56" s="43"/>
+      <c r="CT56" s="43"/>
+      <c r="CU56" s="43"/>
+      <c r="CV56" s="43"/>
+      <c r="CW56" s="43"/>
+      <c r="CX56" s="43"/>
+      <c r="CY56" s="43"/>
     </row>
     <row r="57" spans="1:103" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="45"/>
-      <c r="B57" s="75"/>
-      <c r="C57" s="45"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="45"/>
-      <c r="J57" s="45"/>
-      <c r="K57" s="45"/>
-      <c r="L57" s="45"/>
-      <c r="M57" s="45"/>
-      <c r="N57" s="45"/>
-      <c r="O57" s="45"/>
-      <c r="P57" s="45"/>
-      <c r="Q57" s="45"/>
-      <c r="R57" s="45"/>
-      <c r="S57" s="45"/>
-      <c r="T57" s="45"/>
-      <c r="U57" s="45"/>
-      <c r="V57" s="45"/>
-      <c r="W57" s="45"/>
-      <c r="X57" s="45"/>
-      <c r="Y57" s="45"/>
-      <c r="Z57" s="45"/>
-      <c r="AA57" s="45"/>
-      <c r="AB57" s="45"/>
-      <c r="AC57" s="45"/>
-      <c r="AD57" s="45"/>
-      <c r="AE57" s="45"/>
-      <c r="AF57" s="45"/>
-      <c r="AG57" s="45"/>
-      <c r="AH57" s="45"/>
-      <c r="AI57" s="45"/>
-      <c r="AJ57" s="45"/>
-      <c r="AK57" s="45"/>
-      <c r="AL57" s="45"/>
-      <c r="AM57" s="45"/>
-      <c r="AN57" s="45"/>
-      <c r="AO57" s="45"/>
-      <c r="AP57" s="45"/>
-      <c r="AQ57" s="45"/>
-      <c r="AR57" s="45"/>
-      <c r="AS57" s="45"/>
-      <c r="AT57" s="45"/>
-      <c r="AU57" s="45"/>
-      <c r="AV57" s="45"/>
-      <c r="AW57" s="45"/>
-      <c r="AX57" s="45"/>
-      <c r="AY57" s="45"/>
-      <c r="AZ57" s="45"/>
-      <c r="BA57" s="45"/>
-      <c r="BB57" s="45"/>
-      <c r="BC57" s="45"/>
-      <c r="BD57" s="45"/>
-      <c r="BE57" s="45"/>
-      <c r="BF57" s="45"/>
-      <c r="BG57" s="45"/>
-      <c r="BH57" s="45"/>
-      <c r="BI57" s="45"/>
-      <c r="BJ57" s="45"/>
-      <c r="BK57" s="45"/>
-      <c r="BL57" s="45"/>
-      <c r="BM57" s="45"/>
-      <c r="BN57" s="45"/>
-      <c r="BO57" s="45"/>
-      <c r="BP57" s="45"/>
-      <c r="BQ57" s="45"/>
-      <c r="BR57" s="45"/>
-      <c r="BS57" s="45"/>
-      <c r="BT57" s="45"/>
-      <c r="BU57" s="45"/>
-      <c r="BV57" s="45"/>
-      <c r="BW57" s="45"/>
-      <c r="BX57" s="45"/>
-      <c r="BY57" s="45"/>
-      <c r="BZ57" s="45"/>
-      <c r="CA57" s="45"/>
-      <c r="CB57" s="45"/>
-      <c r="CC57" s="45"/>
-      <c r="CD57" s="45"/>
-      <c r="CE57" s="45"/>
-      <c r="CF57" s="45"/>
-      <c r="CG57" s="45"/>
-      <c r="CH57" s="45"/>
-      <c r="CI57" s="45"/>
-      <c r="CJ57" s="45"/>
-      <c r="CK57" s="45"/>
-      <c r="CL57" s="45"/>
-      <c r="CM57" s="45"/>
-      <c r="CN57" s="45"/>
-      <c r="CO57" s="45"/>
-      <c r="CP57" s="45"/>
-      <c r="CQ57" s="45"/>
-      <c r="CR57" s="45"/>
-      <c r="CS57" s="45"/>
-      <c r="CT57" s="45"/>
-      <c r="CU57" s="45"/>
-      <c r="CV57" s="45"/>
-      <c r="CW57" s="45"/>
-      <c r="CX57" s="45"/>
-      <c r="CY57" s="45"/>
+      <c r="A57" s="43"/>
+      <c r="B57" s="73"/>
+      <c r="C57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="43"/>
+      <c r="K57" s="43"/>
+      <c r="L57" s="43"/>
+      <c r="M57" s="43"/>
+      <c r="N57" s="43"/>
+      <c r="O57" s="43"/>
+      <c r="P57" s="43"/>
+      <c r="Q57" s="43"/>
+      <c r="R57" s="43"/>
+      <c r="S57" s="43"/>
+      <c r="T57" s="43"/>
+      <c r="U57" s="43"/>
+      <c r="V57" s="43"/>
+      <c r="W57" s="43"/>
+      <c r="X57" s="43"/>
+      <c r="Y57" s="43"/>
+      <c r="Z57" s="43"/>
+      <c r="AA57" s="43"/>
+      <c r="AB57" s="43"/>
+      <c r="AC57" s="43"/>
+      <c r="AD57" s="43"/>
+      <c r="AE57" s="43"/>
+      <c r="AF57" s="43"/>
+      <c r="AG57" s="43"/>
+      <c r="AH57" s="43"/>
+      <c r="AI57" s="43"/>
+      <c r="AJ57" s="43"/>
+      <c r="AK57" s="43"/>
+      <c r="AL57" s="43"/>
+      <c r="AM57" s="43"/>
+      <c r="AN57" s="43"/>
+      <c r="AO57" s="43"/>
+      <c r="AP57" s="43"/>
+      <c r="AQ57" s="43"/>
+      <c r="AR57" s="43"/>
+      <c r="AS57" s="43"/>
+      <c r="AT57" s="43"/>
+      <c r="AU57" s="43"/>
+      <c r="AV57" s="43"/>
+      <c r="AW57" s="43"/>
+      <c r="AX57" s="43"/>
+      <c r="AY57" s="43"/>
+      <c r="AZ57" s="43"/>
+      <c r="BA57" s="43"/>
+      <c r="BB57" s="43"/>
+      <c r="BC57" s="43"/>
+      <c r="BD57" s="43"/>
+      <c r="BE57" s="43"/>
+      <c r="BF57" s="43"/>
+      <c r="BG57" s="43"/>
+      <c r="BH57" s="43"/>
+      <c r="BI57" s="43"/>
+      <c r="BJ57" s="43"/>
+      <c r="BK57" s="43"/>
+      <c r="BL57" s="43"/>
+      <c r="BM57" s="43"/>
+      <c r="BN57" s="43"/>
+      <c r="BO57" s="43"/>
+      <c r="BP57" s="43"/>
+      <c r="BQ57" s="43"/>
+      <c r="BR57" s="43"/>
+      <c r="BS57" s="43"/>
+      <c r="BT57" s="43"/>
+      <c r="BU57" s="43"/>
+      <c r="BV57" s="43"/>
+      <c r="BW57" s="43"/>
+      <c r="BX57" s="43"/>
+      <c r="BY57" s="43"/>
+      <c r="BZ57" s="43"/>
+      <c r="CA57" s="43"/>
+      <c r="CB57" s="43"/>
+      <c r="CC57" s="43"/>
+      <c r="CD57" s="43"/>
+      <c r="CE57" s="43"/>
+      <c r="CF57" s="43"/>
+      <c r="CG57" s="43"/>
+      <c r="CH57" s="43"/>
+      <c r="CI57" s="43"/>
+      <c r="CJ57" s="43"/>
+      <c r="CK57" s="43"/>
+      <c r="CL57" s="43"/>
+      <c r="CM57" s="43"/>
+      <c r="CN57" s="43"/>
+      <c r="CO57" s="43"/>
+      <c r="CP57" s="43"/>
+      <c r="CQ57" s="43"/>
+      <c r="CR57" s="43"/>
+      <c r="CS57" s="43"/>
+      <c r="CT57" s="43"/>
+      <c r="CU57" s="43"/>
+      <c r="CV57" s="43"/>
+      <c r="CW57" s="43"/>
+      <c r="CX57" s="43"/>
+      <c r="CY57" s="43"/>
     </row>
     <row r="58" spans="1:103" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="45"/>
-      <c r="B58" s="75"/>
-      <c r="C58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="45"/>
-      <c r="J58" s="45"/>
-      <c r="K58" s="45"/>
-      <c r="L58" s="45"/>
-      <c r="M58" s="45"/>
-      <c r="N58" s="45"/>
-      <c r="O58" s="45"/>
-      <c r="P58" s="45"/>
-      <c r="Q58" s="45"/>
-      <c r="R58" s="45"/>
-      <c r="S58" s="45"/>
-      <c r="T58" s="45"/>
-      <c r="U58" s="45"/>
-      <c r="V58" s="45"/>
-      <c r="W58" s="45"/>
-      <c r="X58" s="45"/>
-      <c r="Y58" s="45"/>
-      <c r="Z58" s="45"/>
-      <c r="AA58" s="45"/>
-      <c r="AB58" s="45"/>
-      <c r="AC58" s="45"/>
-      <c r="AD58" s="45"/>
-      <c r="AE58" s="45"/>
-      <c r="AF58" s="45"/>
-      <c r="AG58" s="45"/>
-      <c r="AH58" s="45"/>
-      <c r="AI58" s="45"/>
-      <c r="AJ58" s="45"/>
-      <c r="AK58" s="45"/>
-      <c r="AL58" s="45"/>
-      <c r="AM58" s="45"/>
-      <c r="AN58" s="45"/>
-      <c r="AO58" s="45"/>
-      <c r="AP58" s="45"/>
-      <c r="AQ58" s="45"/>
-      <c r="AR58" s="45"/>
-      <c r="AS58" s="45"/>
-      <c r="AT58" s="45"/>
-      <c r="AU58" s="45"/>
-      <c r="AV58" s="45"/>
-      <c r="AW58" s="45"/>
-      <c r="AX58" s="45"/>
-      <c r="AY58" s="45"/>
-      <c r="AZ58" s="45"/>
-      <c r="BA58" s="45"/>
-      <c r="BB58" s="45"/>
-      <c r="BC58" s="45"/>
-      <c r="BD58" s="45"/>
-      <c r="BE58" s="45"/>
-      <c r="BF58" s="45"/>
-      <c r="BG58" s="45"/>
-      <c r="BH58" s="45"/>
-      <c r="BI58" s="45"/>
-      <c r="BJ58" s="45"/>
-      <c r="BK58" s="45"/>
-      <c r="BL58" s="45"/>
-      <c r="BM58" s="45"/>
-      <c r="BN58" s="45"/>
-      <c r="BO58" s="45"/>
-      <c r="BP58" s="45"/>
-      <c r="BQ58" s="45"/>
-      <c r="BR58" s="45"/>
-      <c r="BS58" s="45"/>
-      <c r="BT58" s="45"/>
-      <c r="BU58" s="45"/>
-      <c r="BV58" s="45"/>
-      <c r="BW58" s="45"/>
-      <c r="BX58" s="45"/>
-      <c r="BY58" s="45"/>
-      <c r="BZ58" s="45"/>
-      <c r="CA58" s="45"/>
-      <c r="CB58" s="45"/>
-      <c r="CC58" s="45"/>
-      <c r="CD58" s="45"/>
-      <c r="CE58" s="45"/>
-      <c r="CF58" s="45"/>
-      <c r="CG58" s="45"/>
-      <c r="CH58" s="45"/>
-      <c r="CI58" s="45"/>
-      <c r="CJ58" s="45"/>
-      <c r="CK58" s="45"/>
-      <c r="CL58" s="45"/>
-      <c r="CM58" s="45"/>
-      <c r="CN58" s="45"/>
-      <c r="CO58" s="45"/>
-      <c r="CP58" s="45"/>
-      <c r="CQ58" s="45"/>
-      <c r="CR58" s="45"/>
-      <c r="CS58" s="45"/>
-      <c r="CT58" s="45"/>
-      <c r="CU58" s="45"/>
-      <c r="CV58" s="45"/>
-      <c r="CW58" s="45"/>
-      <c r="CX58" s="45"/>
-      <c r="CY58" s="45"/>
+      <c r="A58" s="43"/>
+      <c r="B58" s="73"/>
+      <c r="C58" s="43"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="43"/>
+      <c r="H58" s="43"/>
+      <c r="I58" s="43"/>
+      <c r="J58" s="43"/>
+      <c r="K58" s="43"/>
+      <c r="L58" s="43"/>
+      <c r="M58" s="43"/>
+      <c r="N58" s="43"/>
+      <c r="O58" s="43"/>
+      <c r="P58" s="43"/>
+      <c r="Q58" s="43"/>
+      <c r="R58" s="43"/>
+      <c r="S58" s="43"/>
+      <c r="T58" s="43"/>
+      <c r="U58" s="43"/>
+      <c r="V58" s="43"/>
+      <c r="W58" s="43"/>
+      <c r="X58" s="43"/>
+      <c r="Y58" s="43"/>
+      <c r="Z58" s="43"/>
+      <c r="AA58" s="43"/>
+      <c r="AB58" s="43"/>
+      <c r="AC58" s="43"/>
+      <c r="AD58" s="43"/>
+      <c r="AE58" s="43"/>
+      <c r="AF58" s="43"/>
+      <c r="AG58" s="43"/>
+      <c r="AH58" s="43"/>
+      <c r="AI58" s="43"/>
+      <c r="AJ58" s="43"/>
+      <c r="AK58" s="43"/>
+      <c r="AL58" s="43"/>
+      <c r="AM58" s="43"/>
+      <c r="AN58" s="43"/>
+      <c r="AO58" s="43"/>
+      <c r="AP58" s="43"/>
+      <c r="AQ58" s="43"/>
+      <c r="AR58" s="43"/>
+      <c r="AS58" s="43"/>
+      <c r="AT58" s="43"/>
+      <c r="AU58" s="43"/>
+      <c r="AV58" s="43"/>
+      <c r="AW58" s="43"/>
+      <c r="AX58" s="43"/>
+      <c r="AY58" s="43"/>
+      <c r="AZ58" s="43"/>
+      <c r="BA58" s="43"/>
+      <c r="BB58" s="43"/>
+      <c r="BC58" s="43"/>
+      <c r="BD58" s="43"/>
+      <c r="BE58" s="43"/>
+      <c r="BF58" s="43"/>
+      <c r="BG58" s="43"/>
+      <c r="BH58" s="43"/>
+      <c r="BI58" s="43"/>
+      <c r="BJ58" s="43"/>
+      <c r="BK58" s="43"/>
+      <c r="BL58" s="43"/>
+      <c r="BM58" s="43"/>
+      <c r="BN58" s="43"/>
+      <c r="BO58" s="43"/>
+      <c r="BP58" s="43"/>
+      <c r="BQ58" s="43"/>
+      <c r="BR58" s="43"/>
+      <c r="BS58" s="43"/>
+      <c r="BT58" s="43"/>
+      <c r="BU58" s="43"/>
+      <c r="BV58" s="43"/>
+      <c r="BW58" s="43"/>
+      <c r="BX58" s="43"/>
+      <c r="BY58" s="43"/>
+      <c r="BZ58" s="43"/>
+      <c r="CA58" s="43"/>
+      <c r="CB58" s="43"/>
+      <c r="CC58" s="43"/>
+      <c r="CD58" s="43"/>
+      <c r="CE58" s="43"/>
+      <c r="CF58" s="43"/>
+      <c r="CG58" s="43"/>
+      <c r="CH58" s="43"/>
+      <c r="CI58" s="43"/>
+      <c r="CJ58" s="43"/>
+      <c r="CK58" s="43"/>
+      <c r="CL58" s="43"/>
+      <c r="CM58" s="43"/>
+      <c r="CN58" s="43"/>
+      <c r="CO58" s="43"/>
+      <c r="CP58" s="43"/>
+      <c r="CQ58" s="43"/>
+      <c r="CR58" s="43"/>
+      <c r="CS58" s="43"/>
+      <c r="CT58" s="43"/>
+      <c r="CU58" s="43"/>
+      <c r="CV58" s="43"/>
+      <c r="CW58" s="43"/>
+      <c r="CX58" s="43"/>
+      <c r="CY58" s="43"/>
     </row>
     <row r="59" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D59" s="133"/>
+      <c r="D59" s="131"/>
     </row>
     <row r="60" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="78" t="s">
+      <c r="A60" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="B60" s="75"/>
-      <c r="C60" s="76" t="s">
+      <c r="B60" s="73"/>
+      <c r="C60" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="D60" s="79"/>
-      <c r="E60" s="79"/>
+      <c r="D60" s="77"/>
+      <c r="E60" s="77"/>
     </row>
     <row r="61" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="45"/>
-      <c r="B61" s="75"/>
-      <c r="C61" s="76"/>
-      <c r="D61" s="79"/>
-      <c r="E61" s="45"/>
+      <c r="A61" s="43"/>
+      <c r="B61" s="73"/>
+      <c r="C61" s="74"/>
+      <c r="D61" s="77"/>
+      <c r="E61" s="43"/>
     </row>
     <row r="62" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="45" t="s">
+      <c r="A62" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B62" s="75"/>
-      <c r="C62" s="45" t="s">
+      <c r="B62" s="73"/>
+      <c r="C62" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D62" s="100"/>
-      <c r="E62" s="45"/>
+      <c r="D62" s="98"/>
+      <c r="E62" s="43"/>
     </row>
     <row r="63" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="45"/>
-      <c r="B63" s="75"/>
-      <c r="C63" s="45"/>
-      <c r="D63" s="77"/>
-      <c r="E63" s="45"/>
+      <c r="A63" s="43"/>
+      <c r="B63" s="73"/>
+      <c r="C63" s="43"/>
+      <c r="D63" s="75"/>
+      <c r="E63" s="43"/>
     </row>
     <row r="64" spans="1:103" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="45"/>
-      <c r="B64" s="75"/>
-      <c r="C64" s="45"/>
-      <c r="D64" s="100"/>
-      <c r="E64" s="45"/>
+      <c r="A64" s="43"/>
+      <c r="B64" s="73"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="98"/>
+      <c r="E64" s="43"/>
     </row>
     <row r="65" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="45"/>
-      <c r="B65" s="75"/>
-      <c r="C65" s="45"/>
-      <c r="D65" s="77"/>
-      <c r="E65" s="45"/>
+      <c r="A65" s="43"/>
+      <c r="B65" s="73"/>
+      <c r="C65" s="43"/>
+      <c r="D65" s="75"/>
+      <c r="E65" s="43"/>
     </row>
     <row r="66" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="45"/>
-      <c r="B66" s="75"/>
-      <c r="C66" s="45"/>
-      <c r="D66" s="100"/>
-      <c r="E66" s="45"/>
+      <c r="A66" s="43"/>
+      <c r="B66" s="73"/>
+      <c r="C66" s="43"/>
+      <c r="D66" s="98"/>
+      <c r="E66" s="43"/>
     </row>
     <row r="76" spans="1:5" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3768,27 +3772,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="11.140625" style="87" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="87"/>
+    <col min="1" max="8" width="11.140625" style="85" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="85"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="80"/>
-      <c r="D1" s="82" t="s">
+    <row r="1" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="78"/>
+      <c r="D1" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="F1" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="84"/>
-      <c r="H1" s="85">
+      <c r="G1" s="82"/>
+      <c r="H1" s="83">
         <f>'En-tête'!F5</f>
         <v>0</v>
       </c>
-      <c r="I1" s="85"/>
-      <c r="N1" s="86"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="85"/>
+      <c r="I1" s="83"/>
+      <c r="N1" s="84"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3945,12 +3949,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4119,15 +4120,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8534C3E6-3099-47F9-8B03-0EBDF0F03913}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A333848-59BB-40E8-9C6B-EB280D704CD3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="b1338d7f-541f-4bc8-84bc-74292fa164fd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4152,18 +4165,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A333848-59BB-40E8-9C6B-EB280D704CD3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8534C3E6-3099-47F9-8B03-0EBDF0F03913}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b1338d7f-541f-4bc8-84bc-74292fa164fd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>